<commit_message>
Started QC of match results in `artery_tcl`
</commit_message>
<xml_diff>
--- a/conflation_accuracy.xlsx
+++ b/conflation_accuracy.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="30">
   <si>
     <t>Automatic Traffic Recorders (ATRs)</t>
   </si>
@@ -103,9 +103,6 @@
     <t>random sample of 130 (assumed response distribution of 90%, 5% MOE, 95% LOC)</t>
   </si>
   <si>
-    <t>random sample of 106 (assumed response distribution of 90%, 5% MOE, 95% LOC)</t>
-  </si>
-  <si>
     <t>random sample of 95 (assumed response distribution of 90%, 5% MOE, 95% LOC)</t>
   </si>
   <si>
@@ -113,12 +110,21 @@
   </si>
   <si>
     <t>random sample of 189 intersections (assumed repsonse distribution of 85%, 5% MOE, 95% LOC)</t>
+  </si>
+  <si>
+    <t>Doesn’t exist in TCL boundary</t>
+  </si>
+  <si>
+    <t>random sample of 102 (assumed response distribution of 90%, 5% MOE, 95% LOC)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0%"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -167,7 +173,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -205,16 +211,15 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -497,10 +502,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:J21"/>
+  <dimension ref="A2:J22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -545,13 +550,13 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="15"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="16"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="15"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="5">
@@ -563,12 +568,13 @@
       <c r="C6" s="7">
         <v>17842</v>
       </c>
-      <c r="D6" s="17">
-        <v>0.9</v>
+      <c r="D6" s="18">
+        <f>72/73</f>
+        <v>0.98630136986301364</v>
       </c>
       <c r="E6" s="3" t="str">
-        <f xml:space="preserve"> "random sample of 138 (assumed response distribution of 90%, 5% margin of error, 95% LOC)"</f>
-        <v>random sample of 138 (assumed response distribution of 90%, 5% margin of error, 95% LOC)</v>
+        <f xml:space="preserve"> "random sample of 73 (assumed response distribution of 90%, 5% margin of error, 95% LOC)"</f>
+        <v>random sample of 73 (assumed response distribution of 90%, 5% margin of error, 95% LOC)</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
@@ -581,7 +587,7 @@
       <c r="C7" s="7">
         <v>1968</v>
       </c>
-      <c r="D7" s="17">
+      <c r="D7" s="18">
         <v>0.9</v>
       </c>
       <c r="E7" s="3" t="s">
@@ -590,212 +596,226 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="5">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="C8" s="7">
-        <v>442</v>
-      </c>
-      <c r="D8" s="17">
-        <v>0.9</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>25</v>
+        <v>44</v>
+      </c>
+      <c r="D8" s="18">
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="5">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C9" s="7">
-        <v>296</v>
-      </c>
-      <c r="D9" s="17">
+        <v>380</v>
+      </c>
+      <c r="D9" s="18">
         <v>0.9</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C10" s="7">
-        <v>98</v>
-      </c>
-      <c r="D10" s="17">
-        <v>1</v>
+        <v>300</v>
+      </c>
+      <c r="D10" s="18">
+        <v>0.9</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="J10" s="2"/>
+        <v>25</v>
+      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="5">
+        <v>4</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="7">
+        <v>128</v>
+      </c>
+      <c r="D11" s="18">
+        <v>1</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J11" s="2"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="5">
         <v>5</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B12" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="7">
+      <c r="C12" s="7">
         <v>48</v>
       </c>
-      <c r="D11" s="17">
+      <c r="D12" s="18">
         <v>1</v>
       </c>
-      <c r="E11" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12" s="5" t="s">
+      <c r="E12" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="7">
-        <v>74</v>
-      </c>
-      <c r="D12" s="17">
+      <c r="C13" s="7">
+        <v>60</v>
+      </c>
+      <c r="D13" s="18">
         <v>1</v>
       </c>
-      <c r="E12" s="18" t="s">
+      <c r="E13" s="16" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A13" s="10" t="s">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="10"/>
-      <c r="C13" s="11">
-        <f>SUM(C6:C12)</f>
-        <v>20768</v>
-      </c>
-      <c r="D13" s="20">
-        <f>SUMPRODUCT(C6:C12, D6:D12)/C13</f>
-        <v>0.90105932203389838</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A14" s="15" t="s">
+      <c r="B14" s="10"/>
+      <c r="C14" s="11">
+        <f>SUM(C6:C13)</f>
+        <v>20770</v>
+      </c>
+      <c r="D14" s="19">
+        <f>SUMPRODUCT(C6:C13, D6:D13)/C14</f>
+        <v>0.97548334333634523</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="15"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="16"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A15" s="5">
-        <v>6</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C15" s="8">
-        <v>4691</v>
-      </c>
-      <c r="D15" s="19">
-        <v>0.85</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>28</v>
-      </c>
+      <c r="B15" s="17"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="15"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="5">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C16" s="8">
-        <v>129</v>
-      </c>
-      <c r="D16" s="19">
-        <v>1</v>
+        <v>4664</v>
+      </c>
+      <c r="D16" s="18">
+        <v>0.85</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="5">
+        <v>7</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="8">
+        <v>114</v>
+      </c>
+      <c r="D17" s="18">
+        <v>1</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A18" s="5">
         <v>8</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B18" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="8">
-        <v>97</v>
-      </c>
-      <c r="D17" s="19">
+      <c r="C18" s="8">
+        <v>98</v>
+      </c>
+      <c r="D18" s="18">
         <v>1</v>
       </c>
-      <c r="E17" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="5" t="s">
+      <c r="E18" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B19" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C18" s="8">
+      <c r="C19" s="8">
+        <v>40</v>
+      </c>
+      <c r="D19" s="18">
         <v>1</v>
       </c>
-      <c r="D18" s="17">
-        <v>1</v>
-      </c>
-      <c r="E18" s="18" t="s">
+      <c r="E19" s="16" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="2" t="s">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="2"/>
-      <c r="C19" s="9">
-        <f>SUM(C15:C18)</f>
-        <v>4918</v>
-      </c>
-      <c r="D19" s="20">
-        <f>SUMPRODUCT(C15:C18,D15:D18)/C19</f>
-        <v>0.85692354615697441</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="2" t="s">
+      <c r="B20" s="2"/>
+      <c r="C20" s="9">
+        <f>SUM(C16:C19)</f>
+        <v>4916</v>
+      </c>
+      <c r="D20" s="19">
+        <f>SUMPRODUCT(C16:C19,D16:D19)/C20</f>
+        <v>0.85768917819365331</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="9">
-        <f>C19+C13</f>
+      <c r="C22" s="9">
+        <f>C20+C14</f>
         <v>25686</v>
       </c>
-      <c r="D21" s="20">
-        <f>(C19*D19+C13*D13)/C21</f>
-        <v>0.8926088141399986</v>
+      <c r="D22" s="19">
+        <f>(C20*D20+C14*D14)/C22</f>
+        <v>0.95293891774102191</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A5:D5"/>
-    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="A15:C15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Conflation Accuracy QA/QC Update
</commit_message>
<xml_diff>
--- a/conflation_accuracy.xlsx
+++ b/conflation_accuracy.xlsx
@@ -100,15 +100,9 @@
     <t>check all</t>
   </si>
   <si>
-    <t>random sample of 189 intersections (assumed repsonse distribution of 85%, 5% MOE, 95% LOC)</t>
-  </si>
-  <si>
     <t>Doesn’t exist in TCL boundary</t>
   </si>
   <si>
-    <t>random sample of 102 (assumed response distribution of 90%, 5% MOE, 95% LOC)</t>
-  </si>
-  <si>
     <t>random sample of 71 (assumed response distribution of 95%, 5% MOE, 95% LOC)</t>
   </si>
   <si>
@@ -116,6 +110,12 @@
   </si>
   <si>
     <t>random sample of 95 (assumed response distribution of 90%, 5% MOE, 95% LOC)</t>
+  </si>
+  <si>
+    <t>random sample of 135 intersections (assumed repsonse distribution of 85%, 5% MOE, 95% LOC)</t>
+  </si>
+  <si>
+    <t>random sample of 130 (assumed response distribution of 85%, 5% MOE, 95% LOC)</t>
   </si>
 </sst>
 </file>
@@ -505,7 +505,7 @@
   <dimension ref="A2:J22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -569,8 +569,8 @@
         <v>17842</v>
       </c>
       <c r="D6" s="17">
-        <f>72/73</f>
-        <v>0.98630136986301364</v>
+        <f>73/73</f>
+        <v>1</v>
       </c>
       <c r="E6" s="3" t="str">
         <f xml:space="preserve"> "random sample of 73 (assumed response distribution of 95%, 5% margin of error, 95% LOC)"</f>
@@ -592,7 +592,7 @@
         <v>0.95945945945945943</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
@@ -600,7 +600,7 @@
         <v>11</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C8" s="7">
         <v>44</v>
@@ -620,10 +620,11 @@
         <v>380</v>
       </c>
       <c r="D9" s="17">
-        <v>0.9</v>
+        <f>115/121</f>
+        <v>0.95041322314049592</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
@@ -641,7 +642,7 @@
         <v>0.91578947368421049</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
@@ -693,7 +694,7 @@
         <v>1</v>
       </c>
       <c r="E13" s="16" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
@@ -707,7 +708,7 @@
       </c>
       <c r="D14" s="18">
         <f>SUMPRODUCT(C6:C13, D6:D13)/C14</f>
-        <v>0.98134531051600238</v>
+        <v>0.99403515084809191</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
@@ -730,10 +731,10 @@
         <v>4664</v>
       </c>
       <c r="D16" s="17">
-        <v>0.85</v>
+        <v>0.9</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
@@ -784,7 +785,7 @@
         <v>1</v>
       </c>
       <c r="E19" s="16" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
@@ -798,7 +799,7 @@
       </c>
       <c r="D20" s="18">
         <f>SUMPRODUCT(C16:C19,D16:D19)/C20</f>
-        <v>0.85768917819365331</v>
+        <v>0.90512611879576899</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
@@ -811,7 +812,7 @@
       </c>
       <c r="D22" s="18">
         <f>(C20*D20+C14*D14)/C22</f>
-        <v>0.95767897295870785</v>
+        <v>0.97701900191212609</v>
       </c>
     </row>
   </sheetData>

</xml_diff>